<commit_message>
monday 6.12 from sfr
</commit_message>
<xml_diff>
--- a/covid_read/covid_cases.xlsx
+++ b/covid_read/covid_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timothee\Desktop\auto\covid_read\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bronner\Desktop\Automatization\covid_read\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A3E8A9-975B-4EFE-81B4-1366DD383BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E9F8F6-B4FD-43EB-AB51-C5346D9F07F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid_cases" sheetId="1" r:id="rId1"/>
@@ -870,15 +870,15 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>44529</v>
       </c>
@@ -886,7 +886,7 @@
         <v>19402</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44530</v>
       </c>
@@ -894,7 +894,7 @@
         <v>8422</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44531</v>
       </c>
@@ -903,7 +903,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44532</v>
       </c>
@@ -911,7 +911,7 @@
         <v>9546</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44533</v>
       </c>
@@ -919,160 +919,163 @@
         <v>9951</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44534</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44535</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44536</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>23888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44537</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44538</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44539</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44540</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44541</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44542</v>
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44543</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44544</v>
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44545</v>
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44546</v>
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44547</v>
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44548</v>
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44549</v>
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44550</v>
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44551</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44552</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44553</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44554</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44555</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44556</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44557</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44558</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44559</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44560</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44561</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44562</v>
       </c>

</xml_diff>